<commit_message>
Update .gitignore and enhance funding extractor functionality
- Added log and output file types to .gitignore
- Improved matching logic in find_potential_matches function to return more options for single-word matches
- Updated output file formats from Excel to CSV for funding details and unmatched children reports
- Renamed output files for clarity
</commit_message>
<xml_diff>
--- a/output/children_basic_info.xlsx
+++ b/output/children_basic_info.xlsx
@@ -82,13 +82,13 @@
     <t>Bobby Johnston</t>
   </si>
   <si>
-    <t>Boden Williams</t>
+    <t>Boden Nelson Williams</t>
   </si>
   <si>
     <t>Caelan Jameson</t>
   </si>
   <si>
-    <t>Calum Carroll ward</t>
+    <t>Calum Thomas Carroll Ward</t>
   </si>
   <si>
     <t>Cameron Finn</t>
@@ -97,10 +97,10 @@
     <t>Charlie Jordan</t>
   </si>
   <si>
-    <t>Charlotte Guyler</t>
-  </si>
-  <si>
-    <t>Charlotte Rose Doyle</t>
+    <t>Lottie Charlotte Guyler</t>
+  </si>
+  <si>
+    <t>Charlotte Doyle</t>
   </si>
   <si>
     <t>Cillian Redmond</t>
@@ -130,13 +130,13 @@
     <t>Dylan Hoseason</t>
   </si>
   <si>
-    <t>Eleanor Wadden</t>
+    <t>Eleanor Niamh Wadden</t>
   </si>
   <si>
     <t>Ellis Guyett</t>
   </si>
   <si>
-    <t>Elsie Williams</t>
+    <t>Elsie Nelson Williams</t>
   </si>
   <si>
     <t>Emilia Kearney Collinge</t>
@@ -145,7 +145,7 @@
     <t>Ena Milosevic</t>
   </si>
   <si>
-    <t>Eve Otoole</t>
+    <t>Eve O Toole</t>
   </si>
   <si>
     <t>Farah Hani</t>
@@ -169,7 +169,7 @@
     <t>Jack Farrell</t>
   </si>
   <si>
-    <t>Jack Vickers McGerr</t>
+    <t>JP Vickers McGerr</t>
   </si>
   <si>
     <t>Jacob Corcoran</t>
@@ -184,7 +184,7 @@
     <t>Joshua Soden</t>
   </si>
   <si>
-    <t>Juno Luna Hynes Byrne</t>
+    <t>Juno Hynes Byrne</t>
   </si>
   <si>
     <t>Kabir Sharma</t>
@@ -199,7 +199,7 @@
     <t>Katie Sheehy</t>
   </si>
   <si>
-    <t>Katie Vickers Mc Gerr</t>
+    <t>Katie Mcgerr</t>
   </si>
   <si>
     <t>Kodi O Carroll Scannell</t>
@@ -214,10 +214,10 @@
     <t>Lily Crinnion</t>
   </si>
   <si>
-    <t>Lily Grnik</t>
-  </si>
-  <si>
-    <t>Lily Kathy May Corcoran</t>
+    <t>Lily Gornik</t>
+  </si>
+  <si>
+    <t>Lily Corcoran</t>
   </si>
   <si>
     <t>LILY LACERDA MEDEIROS</t>
@@ -232,7 +232,7 @@
     <t>Maia Liliana Walker Rusu</t>
   </si>
   <si>
-    <t>Marc Aurele Gaaloul Donnelly</t>
+    <t>Marc Gaaloul Donnelly</t>
   </si>
   <si>
     <t>Mason O Donnell</t>
@@ -250,7 +250,7 @@
     <t>Molly Byrne Lucey</t>
   </si>
   <si>
-    <t>Naoise Siochr</t>
+    <t>Naoise O Siochru</t>
   </si>
   <si>
     <t>Nicholas Birgaoanu</t>
@@ -280,7 +280,7 @@
     <t>Rafael McGlynn Roberts</t>
   </si>
   <si>
-    <t>Ray OCleirigh</t>
+    <t>Ray O Cleirigh</t>
   </si>
   <si>
     <t>Ran Doherty</t>
@@ -313,13 +313,13 @@
     <t>Theo Hughes</t>
   </si>
   <si>
-    <t>Theo OShaughnessy</t>
+    <t>Theo O Shaughnessy</t>
   </si>
   <si>
     <t>Tola Jasieniecka</t>
   </si>
   <si>
-    <t>Toms Hobbs</t>
+    <t>Toms Carmody Finnegan</t>
   </si>
   <si>
     <t>Ula OBrien</t>

</xml_diff>